<commit_message>
chore: update intent qna
</commit_message>
<xml_diff>
--- a/packages/test-qna/intents.xlsx
+++ b/packages/test-qna/intents.xlsx
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">Delivery-date</t>
   </si>
   <si>
-    <t xml:space="preserve">If you purchase today before 10pm, you purchase will be delivered by 2018-01-12</t>
-  </si>
-  <si>
     <t xml:space="preserve">When will I receive my parcel?</t>
   </si>
   <si>
@@ -35,6 +32,57 @@
   </si>
   <si>
     <t xml:space="preserve">How long is the delivery?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can pay for your purchase with Visa, Mastercard or using a PayPal account.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can i pay with credit card ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can i pay in bitcoins ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shipping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your purchase can be shipped worldwide. However, delivery charges may vary.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you ship to France ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please reach us at contact@my-sample-compagny.com for further assistance.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A have a problem on the website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invoice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The invoice for your purchase will be sent along with your goods. You can also download an electronic version from your account.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Could you send me an invoice please ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Policy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hello! I can provide you with information about our payment and shipping policies.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I need some help</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can you help me ?</t>
   </si>
 </sst>
 </file>
@@ -49,6 +97,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -108,12 +157,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -134,10 +179,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -151,8 +196,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>1</v>
       </c>
     </row>
@@ -166,9 +211,89 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>